<commit_message>
few approval groups related scripts are added
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/Pre_Requisite.xlsx
+++ b/src/main/resources/Data/Pre_Requisite.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkhare\git\VMS_Automation_TestNG_Cucumber\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF23A58-008F-4FB8-9D21-A110661399C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D63AE5-90C1-423A-A6FE-02CDEC8B6274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2614B4C3-0DE0-494E-9633-EDF4726DB0D6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>ClientID</t>
   </si>
@@ -50,6 +50,48 @@
   </si>
   <si>
     <t>sTestCaseID</t>
+  </si>
+  <si>
+    <t>CalvinDerekAG</t>
+  </si>
+  <si>
+    <t>Calvin Derek</t>
+  </si>
+  <si>
+    <t>ApprovalGroupName</t>
+  </si>
+  <si>
+    <t>ApprovalManager</t>
+  </si>
+  <si>
+    <t>AddApprovalGroupPO_GuideWellGroupInc</t>
+  </si>
+  <si>
+    <t>Primary Owner</t>
+  </si>
+  <si>
+    <t>Dunston</t>
+  </si>
+  <si>
+    <t>AddApprovalGroupPO_SEIT0019</t>
+  </si>
+  <si>
+    <t>Burns &amp; McDonnell</t>
+  </si>
+  <si>
+    <t>Acton Sara</t>
+  </si>
+  <si>
+    <t>AddAutomationGroup_WyndhamWorldwide</t>
+  </si>
+  <si>
+    <t>Wyndham Destinations</t>
+  </si>
+  <si>
+    <t>Automation Group</t>
+  </si>
+  <si>
+    <t>Perez Madalene</t>
   </si>
 </sst>
 </file>
@@ -100,9 +142,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,19 +460,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19F8F07-59A0-485F-A945-2110E9508699}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -439,8 +484,14 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -450,66 +501,126 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3670</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3858</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>392</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>